<commit_message>
Work on V 2.5.9
</commit_message>
<xml_diff>
--- a/Bio_Industries/prototypes/Bio_Farm/Wood-Production.xlsx
+++ b/Bio_Industries/prototypes/Bio_Farm/Wood-Production.xlsx
@@ -312,13 +312,121 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -329,114 +437,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -742,7 +742,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A3"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -754,88 +754,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="24" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="13" t="s">
+      <c r="F1" s="47"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="15"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="51"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="35"/>
-      <c r="B2" s="42" t="s">
+      <c r="A2" s="42"/>
+      <c r="B2" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="43" t="s">
+      <c r="C2" s="41"/>
+      <c r="D2" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="28" t="s">
+      <c r="F2" s="35"/>
+      <c r="G2" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="17" t="s">
+      <c r="I2" s="38"/>
+      <c r="J2" s="39" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" s="35"/>
-      <c r="B3" s="44" t="s">
+      <c r="A3" s="42"/>
+      <c r="B3" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="29" t="s">
+      <c r="D3" s="33"/>
+      <c r="E3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="18" t="s">
+      <c r="G3" s="36"/>
+      <c r="H3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="17"/>
+      <c r="J3" s="39"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="45">
+      <c r="B4" s="26">
         <v>20</v>
       </c>
       <c r="C4" s="4">
         <f>B4*2</f>
         <v>40</v>
       </c>
-      <c r="D4" s="46">
-        <v>100</v>
-      </c>
-      <c r="E4" s="30">
+      <c r="D4" s="27">
+        <v>200</v>
+      </c>
+      <c r="E4" s="17">
         <f>C4/2</f>
         <v>20</v>
       </c>
@@ -843,11 +843,11 @@
         <f>E4*2</f>
         <v>40</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="18">
         <f>D4*2</f>
-        <v>200</v>
-      </c>
-      <c r="H4" s="19">
+        <v>400</v>
+      </c>
+      <c r="H4" s="11">
         <f>F4/2</f>
         <v>20</v>
       </c>
@@ -855,41 +855,41 @@
         <f>H4*2</f>
         <v>40</v>
       </c>
-      <c r="J4" s="20">
-        <f>G4*2</f>
+      <c r="J4" s="12">
+        <f>G4</f>
         <v>400</v>
       </c>
       <c r="L4">
         <f>J4+G4+D4</f>
-        <v>700</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="45">
+      <c r="B5" s="26">
         <v>20</v>
       </c>
       <c r="C5" s="4">
         <f>B5*2.5</f>
         <v>50</v>
       </c>
-      <c r="D5" s="46">
-        <v>90</v>
-      </c>
-      <c r="E5" s="30">
+      <c r="D5" s="27">
+        <v>150</v>
+      </c>
+      <c r="E5" s="17">
         <f t="shared" ref="E5:E7" si="0">C5/2</f>
         <v>25</v>
       </c>
       <c r="F5" s="3">
         <v>60</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="18">
         <f t="shared" ref="G5:G7" si="1">D5*2</f>
-        <v>180</v>
-      </c>
-      <c r="H5" s="19">
+        <v>300</v>
+      </c>
+      <c r="H5" s="11">
         <f t="shared" ref="H5:H7" si="2">F5/2</f>
         <v>30</v>
       </c>
@@ -897,30 +897,29 @@
         <f>H5*2.5</f>
         <v>75</v>
       </c>
-      <c r="J5" s="20">
-        <f t="shared" ref="J5:J7" si="3">G5*2</f>
+      <c r="J5" s="12">
         <v>360</v>
       </c>
       <c r="L5">
-        <f t="shared" ref="L5:L7" si="4">J5+G5+D5</f>
-        <v>630</v>
+        <f t="shared" ref="L5:L7" si="3">J5+G5+D5</f>
+        <v>810</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="47">
+      <c r="B6" s="28">
         <v>20</v>
       </c>
-      <c r="C6" s="48">
+      <c r="C6" s="29">
         <f>B6*3</f>
         <v>60</v>
       </c>
-      <c r="D6" s="49">
-        <v>75</v>
-      </c>
-      <c r="E6" s="30">
+      <c r="D6" s="30">
+        <v>100</v>
+      </c>
+      <c r="E6" s="17">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
@@ -928,11 +927,11 @@
         <f>E6*3</f>
         <v>90</v>
       </c>
-      <c r="G6" s="31">
+      <c r="G6" s="18">
         <f t="shared" si="1"/>
-        <v>150</v>
-      </c>
-      <c r="H6" s="19">
+        <v>200</v>
+      </c>
+      <c r="H6" s="11">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
@@ -940,70 +939,69 @@
         <f>H6*3</f>
         <v>135</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="12">
+        <v>300</v>
+      </c>
+      <c r="L6">
         <f t="shared" si="3"/>
-        <v>300</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="4"/>
-        <v>525</v>
+        <v>600</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="51" t="s">
+      <c r="A7" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="36">
+      <c r="B7" s="22">
         <v>20</v>
       </c>
-      <c r="C7" s="37">
+      <c r="C7" s="23">
         <f>B7*4</f>
         <v>80</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="24">
         <v>50</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="19">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="20">
         <f>E7*4</f>
         <v>160</v>
       </c>
-      <c r="G7" s="34">
+      <c r="G7" s="21">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="13">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7" s="14">
         <f>H7*4</f>
         <v>320</v>
       </c>
-      <c r="J7" s="23">
+      <c r="J7" s="15">
+        <f t="shared" ref="J5:J7" si="4">G7*2</f>
+        <v>200</v>
+      </c>
+      <c r="L7">
         <f t="shared" si="3"/>
-        <v>200</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="4"/>
         <v>350</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:J3"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>